<commit_message>
feat: update the label, comment, description in the template file
update the label, comment, description in the template file
</commit_message>
<xml_diff>
--- a/template/SHACL-agent.xlsx
+++ b/template/SHACL-agent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaofengliao/Documents/HealthRI/SchaclV2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaofengliao/Documents/HealthRI/excel2rdf/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F3EBB-15A7-0442-9B5D-8FB5DD9BA9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4CC811-FDF5-B341-A02B-95FD32FA9EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32440" yWindow="9360" windowWidth="28380" windowHeight="18520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="820" windowWidth="28380" windowHeight="18520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prefixes" sheetId="1" r:id="rId1"/>
@@ -355,12 +355,6 @@
     <t>dash:LiteralViewer</t>
   </si>
   <si>
-    <t>Excel template for Agent class</t>
-  </si>
-  <si>
-    <t>This is an excel template for Agent class in Health RI Core plateau 2.</t>
-  </si>
-  <si>
     <t>http://data.health-ri.nl/core/p2/AgentShape</t>
   </si>
   <si>
@@ -383,6 +377,12 @@
   </si>
   <si>
     <t>example:AgentShape#dct-identifier</t>
+  </si>
+  <si>
+    <t>SHACL of Agent class</t>
+  </si>
+  <si>
+    <t>SHACL of Agent class in Health RI Core plateau 2.</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+    <sheetView zoomScale="95" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +1712,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1734,10 +1734,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1762,7 +1762,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -1780,7 +1780,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -1789,7 +1789,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -1798,7 +1798,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1928,10 +1928,10 @@
     </row>
     <row r="14" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>50</v>
@@ -2009,7 +2009,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4"/>
       <c r="O1" s="4"/>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="8" spans="1:22" s="41" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="42"/>
       <c r="F8" s="43"/>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>110</v>
-      </c>
       <c r="E9" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G9" s="49">
         <v>1</v>
@@ -2232,10 +2232,10 @@
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="50" t="s">
         <v>98</v>
@@ -2277,6 +2277,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc89d7aa5f4d5299fdff9a433ddfde7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1001ca5b3032e4f3d8abb5daa6c8e0f8" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -2530,29 +2552,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D97997-30E9-4CC7-A812-E39596E8A4EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2569,23 +2588,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add properties to agent template to align with v2 diagram
1. Change sh:Literal to rdfs:literal in the agent template. This may failed to pass validation.
2. added several properties to agent template, including foaf_mbox, foaf:homepage, dct:spatial, dct:type, healthdcatap:publisherType, healthdcatap:publisherNote
3. Put the xls2rdf-app-2.2.0-onejar.jar in this folder, convenient to generate shacl. Will be removed later.
</commit_message>
<xml_diff>
--- a/template/SHACL-agent.xlsx
+++ b/template/SHACL-agent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaofengliao/Documents/HealthRI/excel2rdf/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB182785-3DD4-1647-90EA-0442DA77F913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C229BB-DA66-6948-984C-0B78770430BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="820" windowWidth="28380" windowHeight="18520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35720" yWindow="3400" windowWidth="28380" windowHeight="18520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prefixes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="137">
   <si>
     <t>PREFIX</t>
   </si>
@@ -334,9 +334,6 @@
     <t>foaf:Agent</t>
   </si>
   <si>
-    <t>sh:Literal</t>
-  </si>
-  <si>
     <t>dct:identifier</t>
   </si>
   <si>
@@ -383,6 +380,78 @@
   </si>
   <si>
     <t>SHACL of Agent class in Health RI Core plateau 2.</t>
+  </si>
+  <si>
+    <t>rdfs:Literal</t>
+  </si>
+  <si>
+    <t>foaf:mbox</t>
+  </si>
+  <si>
+    <t>Email box</t>
+  </si>
+  <si>
+    <t>sh:IRI</t>
+  </si>
+  <si>
+    <t>dash:URIViewer</t>
+  </si>
+  <si>
+    <t>dash:URIEditor</t>
+  </si>
+  <si>
+    <t>^mailto:.+@.+\\..+$</t>
+  </si>
+  <si>
+    <t>sh:pattern</t>
+  </si>
+  <si>
+    <t>example:AgentShape#foaf-mbox</t>
+  </si>
+  <si>
+    <t>foaf:homepage</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>dct:spatial</t>
+  </si>
+  <si>
+    <t>dct:type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>example:AgentShape#healthdcatap-publisherType</t>
+  </si>
+  <si>
+    <t>example:AgentShape#dct-type</t>
+  </si>
+  <si>
+    <t>example:AgentShape#dct-spatial</t>
+  </si>
+  <si>
+    <t>healthdcatap:publisherType</t>
+  </si>
+  <si>
+    <t>Publisher Type</t>
+  </si>
+  <si>
+    <t>example:AgentShape#healthdcatap-publisherNote</t>
+  </si>
+  <si>
+    <t>healthdcatap:publisherNote</t>
+  </si>
+  <si>
+    <t>Publisher Note</t>
+  </si>
+  <si>
+    <t>example:AgentShape#foaf-homepage</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1198,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1263,6 +1332,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="162">
     <cellStyle name="20 % - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1698,10 +1769,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
         <v>100</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -1712,7 +1783,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
@@ -1762,7 +1833,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -1780,7 +1851,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -1789,7 +1860,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -1798,7 +1869,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1928,10 +1999,10 @@
     </row>
     <row r="14" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>50</v>
@@ -1971,13 +2042,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2004,18 +2075,18 @@
     <col min="1019" max="1023" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="4"/>
       <c r="O1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="3" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>51</v>
       </c>
@@ -2029,12 +2100,12 @@
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D4" s="28"/>
       <c r="G4" s="29"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:22" s="13" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" s="13" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>52</v>
       </c>
@@ -2096,7 +2167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="32" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" s="32" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>72</v>
       </c>
@@ -2118,7 +2189,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
     </row>
-    <row r="7" spans="1:22" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="36" t="s">
         <v>39</v>
       </c>
@@ -2185,10 +2256,13 @@
       <c r="V7" s="47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" s="41" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W7" s="37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="41" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="42"/>
       <c r="F8" s="43"/>
@@ -2198,21 +2272,21 @@
       <c r="S8" s="45"/>
       <c r="T8" s="45"/>
     </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="D9" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="50" t="s">
-        <v>108</v>
-      </c>
       <c r="E9" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="49">
         <v>1</v>
@@ -2221,30 +2295,30 @@
         <v>1</v>
       </c>
       <c r="I9" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="U9" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="V9" s="52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.15">
+      <c r="A10" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="U9" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="V9" s="52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.15">
-      <c r="A10" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="50" t="s">
+      <c r="D10" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>99</v>
-      </c>
       <c r="E10" s="51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="49">
         <v>1</v>
@@ -2253,13 +2327,193 @@
         <v>1</v>
       </c>
       <c r="I10" s="52" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="U10" s="52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V10" s="52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1</v>
+      </c>
+      <c r="H11" s="24">
+        <v>1</v>
+      </c>
+      <c r="I11" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="U11" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="V11" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="W11" s="52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="23">
+        <v>1</v>
+      </c>
+      <c r="H12" s="24">
+        <v>1</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="U12" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="V12" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="U13" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="V13" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="24">
+        <v>1</v>
+      </c>
+      <c r="I14" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="U14" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="V14" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="24">
+        <v>1</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="U15" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="V15" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="24">
+        <v>1</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="U16" s="52" t="s">
         <v>102</v>
+      </c>
+      <c r="V16" s="52" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2277,28 +2531,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc89d7aa5f4d5299fdff9a433ddfde7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1001ca5b3032e4f3d8abb5daa6c8e0f8" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -2552,26 +2784,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D97997-30E9-4CC7-A812-E39596E8A4EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2588,4 +2823,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>